<commit_message>
feat(translation): add D3 translation for pa,as,hi,ml,gu
</commit_message>
<xml_diff>
--- a/utils/localisation_script/excel_to_json/gu/p.xlsx
+++ b/utils/localisation_script/excel_to_json/gu/p.xlsx
@@ -5,24 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umair.manzoor/Projects/Open-Speech-EkStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/gu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/gu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4A7A2F-3F7E-8C42-B692-AAE5DDCAB485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDED3E2-D5B7-024D-B6F9-6842305A9EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20500" windowHeight="7760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delta" sheetId="7" r:id="rId1"/>
     <sheet name="Delta 2" sheetId="8" r:id="rId2"/>
-    <sheet name="Sheet10" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
   <si>
     <t>Heading</t>
   </si>
@@ -82,9 +81,6 @@
   </si>
   <si>
     <t>Page Name</t>
-  </si>
-  <si>
-    <t>English Copy</t>
   </si>
   <si>
     <t>All functional Pages</t>
@@ -355,10 +351,10 @@
     <t>યુઝર બદલો</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gujarati</t>
-  </si>
-  <si>
     <t>Gujarati</t>
+  </si>
+  <si>
+    <t>English copy</t>
   </si>
 </sst>
 </file>
@@ -838,8 +834,8 @@
   </sheetPr>
   <dimension ref="A2:G1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
@@ -862,11 +858,11 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="39" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="F2" s="39"/>
       <c r="G2" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -876,56 +872,56 @@
     </row>
     <row r="4" spans="1:7" ht="14">
       <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="32" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>24</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14">
       <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14">
       <c r="D6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>27</v>
       </c>
       <c r="F6" s="33"/>
       <c r="G6" s="41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="126">
       <c r="D7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="34" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -935,10 +931,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="33"/>
@@ -967,7 +963,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="35">
         <v>1</v>
@@ -980,14 +976,14 @@
     <row r="13" spans="1:7" ht="98">
       <c r="C13" s="4"/>
       <c r="D13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="33"/>
       <c r="G13" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14">
@@ -1000,7 +996,7 @@
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14">
@@ -1008,7 +1004,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="36">
         <v>2</v>
@@ -1021,14 +1017,14 @@
     <row r="16" spans="1:7" ht="98">
       <c r="C16" s="4"/>
       <c r="D16" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14">
@@ -1041,7 +1037,7 @@
       </c>
       <c r="F17" s="33"/>
       <c r="G17" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14">
@@ -1049,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="35">
         <v>3</v>
@@ -1062,14 +1058,14 @@
     <row r="19" spans="1:7" ht="84">
       <c r="C19" s="4"/>
       <c r="D19" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="33"/>
       <c r="G19" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14">
@@ -1082,7 +1078,7 @@
       </c>
       <c r="F20" s="33"/>
       <c r="G20" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14">
@@ -1090,7 +1086,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="35">
         <v>4</v>
@@ -1103,14 +1099,14 @@
     <row r="22" spans="1:7" ht="112">
       <c r="C22" s="4"/>
       <c r="D22" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14">
@@ -1123,7 +1119,7 @@
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1133,20 +1129,20 @@
     </row>
     <row r="25" spans="1:7" ht="14">
       <c r="A25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="32" t="s">
         <v>38</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>39</v>
       </c>
       <c r="F25" s="33"/>
       <c r="G25" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1156,23 +1152,23 @@
     </row>
     <row r="27" spans="1:7" ht="42">
       <c r="D27" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28">
       <c r="E28" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F28" s="33"/>
       <c r="G28" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1185,11 +1181,11 @@
         <v>2</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1199,41 +1195,41 @@
     </row>
     <row r="32" spans="1:7" ht="14">
       <c r="C32" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="38" t="s">
         <v>43</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>44</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:7" ht="14">
       <c r="D33" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="38" t="s">
         <v>45</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>46</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="3:7" ht="28">
       <c r="D34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="38" t="s">
         <v>47</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>48</v>
       </c>
       <c r="F34" s="33"/>
       <c r="G34" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="3:7">
@@ -1243,26 +1239,26 @@
     </row>
     <row r="36" spans="3:7" ht="14">
       <c r="D36" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F36" s="33"/>
       <c r="G36" s="40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="3:7" ht="14">
       <c r="D37" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37" s="33"/>
       <c r="G37" s="40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="3:7">
@@ -1272,26 +1268,26 @@
     </row>
     <row r="39" spans="3:7" ht="14">
       <c r="D39" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F39" s="33"/>
       <c r="G39" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="3:7" ht="14">
       <c r="D40" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F40" s="33"/>
       <c r="G40" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="3:7">
@@ -1301,26 +1297,26 @@
     </row>
     <row r="42" spans="3:7" ht="14">
       <c r="D42" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E42" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F42" s="33"/>
       <c r="G42" s="40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="3:7" ht="28">
       <c r="D43" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="32" t="s">
         <v>54</v>
-      </c>
-      <c r="E43" s="32" t="s">
-        <v>55</v>
       </c>
       <c r="F43" s="33"/>
       <c r="G43" s="41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="3:7">
@@ -1330,17 +1326,17 @@
     </row>
     <row r="45" spans="3:7" ht="14">
       <c r="C45" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E45" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F45" s="33"/>
       <c r="G45" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="3:7">
@@ -4235,8 +4231,8 @@
   </sheetPr>
   <dimension ref="A2:G1001"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
@@ -4258,11 +4254,11 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4270,40 +4266,40 @@
     </row>
     <row r="4" spans="1:7" ht="14">
       <c r="A4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14">
       <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14">
       <c r="D6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="112">
       <c r="D7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4311,13 +4307,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="98">
@@ -4326,7 +4322,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4338,7 +4334,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="8"/>
       <c r="E12" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14">
@@ -4346,17 +4342,17 @@
         <v>9</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="84">
       <c r="C14" s="6"/>
       <c r="D14" s="5"/>
       <c r="E14" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4369,7 +4365,7 @@
         <v>11</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="24">
         <v>1</v>
@@ -4378,10 +4374,10 @@
     <row r="17" spans="1:5" ht="98">
       <c r="C17" s="25"/>
       <c r="D17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14">
@@ -4398,7 +4394,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="15">
         <v>2</v>
@@ -4407,10 +4403,10 @@
     <row r="20" spans="1:5" ht="98">
       <c r="C20" s="25"/>
       <c r="D20" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14">
@@ -4427,7 +4423,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="24">
         <v>3</v>
@@ -4436,10 +4432,10 @@
     <row r="23" spans="1:5" ht="84">
       <c r="C23" s="25"/>
       <c r="D23" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14">
@@ -4456,7 +4452,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="24">
         <v>4</v>
@@ -4465,10 +4461,10 @@
     <row r="26" spans="1:5" ht="112">
       <c r="C26" s="25"/>
       <c r="D26" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14">
@@ -4485,16 +4481,16 @@
     </row>
     <row r="29" spans="1:5" ht="14">
       <c r="A29" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -4502,15 +4498,15 @@
     </row>
     <row r="31" spans="1:5" ht="42">
       <c r="D31" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28">
       <c r="E32" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -4521,7 +4517,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -4529,29 +4525,29 @@
     </row>
     <row r="36" spans="1:5" ht="14">
       <c r="C36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="28" t="s">
         <v>43</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14">
       <c r="D37" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="28" t="s">
         <v>45</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="28">
       <c r="D38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="28" t="s">
         <v>47</v>
-      </c>
-      <c r="E38" s="28" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -4562,13 +4558,13 @@
     </row>
     <row r="41" spans="1:5" ht="14">
       <c r="C41" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -4576,7 +4572,7 @@
     </row>
     <row r="43" spans="1:5" ht="15">
       <c r="A43" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>3</v>
@@ -4585,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30">
@@ -4594,7 +4590,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -4602,10 +4598,10 @@
     </row>
     <row r="46" spans="1:5">
       <c r="D46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -4613,24 +4609,24 @@
     </row>
     <row r="48" spans="1:5" ht="42">
       <c r="C48" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="3:5">
       <c r="C49" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="3:5">
@@ -7492,19 +7488,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>